<commit_message>
incorporacion modelo 1 y 2 flotas
</commit_message>
<xml_diff>
--- a/mod1/Planilla merluza.xlsx
+++ b/mod1/Planilla merluza.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SSmerluza" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="142">
   <si>
     <t xml:space="preserve">Year </t>
   </si>
@@ -194,12 +194,6 @@
   </si>
   <si>
     <t>Nsamp</t>
-  </si>
-  <si>
-    <t>#2019</t>
-  </si>
-  <si>
-    <t>#2020</t>
   </si>
   <si>
     <t>#wt_flt_1</t>
@@ -473,10 +467,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,15 +504,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -781,7 +786,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -799,12 +804,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -812,7 +817,7 @@
         <v>1992</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -820,7 +825,7 @@
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -828,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -836,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -844,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -852,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -860,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -868,7 +873,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -876,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -884,47 +889,47 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -944,10 +949,10 @@
         <v>0.01</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -970,7 +975,7 @@
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -978,64 +983,64 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
         <v>92</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>93</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>94</v>
-      </c>
-      <c r="D32" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1573,30 +1578,30 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" t="s">
         <v>97</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>98</v>
-      </c>
-      <c r="C64" t="s">
-        <v>99</v>
-      </c>
-      <c r="D64" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
         <v>101</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>102</v>
-      </c>
-      <c r="C65" t="s">
-        <v>103</v>
-      </c>
-      <c r="D65" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -1630,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2679,7 +2684,7 @@
         <v>301330</v>
       </c>
       <c r="E113" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F113" t="s">
         <v>34</v>
@@ -2705,7 +2710,7 @@
         <v>35</v>
       </c>
       <c r="G114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -2728,7 +2733,7 @@
         <v>35</v>
       </c>
       <c r="G115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -2751,7 +2756,7 @@
         <v>35</v>
       </c>
       <c r="G116" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -2776,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="B118" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -2784,17 +2789,17 @@
         <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -2802,7 +2807,7 @@
         <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -2810,7 +2815,7 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -2818,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -2826,7 +2831,7 @@
         <v>65</v>
       </c>
       <c r="B125" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -2834,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -2842,12 +2847,12 @@
         <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
@@ -2890,12 +2895,12 @@
         <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2904,7 +2909,7 @@
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.35">
@@ -2991,7 +2996,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B134">
         <v>1.5</v>
@@ -3032,7 +3037,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B135">
         <v>0.65</v>
@@ -3073,42 +3078,42 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.35">
@@ -3160,25 +3165,25 @@
         <v>30</v>
       </c>
       <c r="H145" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B147" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.35">
@@ -6348,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="B200" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.35">
@@ -6356,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="B201" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.35">
@@ -6364,7 +6369,7 @@
         <v>0</v>
       </c>
       <c r="B202" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.35">
@@ -6372,7 +6377,7 @@
         <v>0</v>
       </c>
       <c r="B203" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.35">
@@ -6380,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.35">
@@ -6388,7 +6393,7 @@
         <v>0</v>
       </c>
       <c r="B205" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.35">
@@ -6398,7 +6403,7 @@
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -8801,7 +8806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -13104,20 +13109,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="21" max="21" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
@@ -13131,7 +13139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -13145,7 +13153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -13159,12 +13167,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -13226,7 +13234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1992</v>
       </c>
@@ -13287,8 +13295,9 @@
       <c r="T8">
         <v>3928</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1993</v>
       </c>
@@ -13349,8 +13358,9 @@
       <c r="T9">
         <v>3355</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1994</v>
       </c>
@@ -13411,8 +13421,9 @@
       <c r="T10">
         <v>752</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1995</v>
       </c>
@@ -13473,8 +13484,9 @@
       <c r="T11">
         <v>691</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1996</v>
       </c>
@@ -13535,8 +13547,9 @@
       <c r="T12">
         <v>2144</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1997</v>
       </c>
@@ -13597,8 +13610,9 @@
       <c r="T13">
         <v>289.39999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1998</v>
       </c>
@@ -13659,8 +13673,9 @@
       <c r="T14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1999</v>
       </c>
@@ -13721,8 +13736,9 @@
       <c r="T15">
         <v>199.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2000</v>
       </c>
@@ -13783,8 +13799,9 @@
       <c r="T16">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2001</v>
       </c>
@@ -13845,8 +13862,9 @@
       <c r="T17">
         <v>248.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2002</v>
       </c>
@@ -13907,8 +13925,9 @@
       <c r="T18">
         <v>1928.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -13969,8 +13988,9 @@
       <c r="T19">
         <v>5520.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -14031,8 +14051,9 @@
       <c r="T20">
         <v>835.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2005</v>
       </c>
@@ -14093,8 +14114,9 @@
       <c r="T21">
         <v>390.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2006</v>
       </c>
@@ -14155,8 +14177,9 @@
       <c r="T22">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2007</v>
       </c>
@@ -14217,8 +14240,9 @@
       <c r="T23">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2008</v>
       </c>
@@ -14279,8 +14303,9 @@
       <c r="T24">
         <v>265.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2009</v>
       </c>
@@ -14341,8 +14366,9 @@
       <c r="T25">
         <v>69.599999999999994</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2010</v>
       </c>
@@ -14403,8 +14429,9 @@
       <c r="T26">
         <v>339.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2011</v>
       </c>
@@ -14465,8 +14492,9 @@
       <c r="T27">
         <v>520.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2012</v>
       </c>
@@ -14527,8 +14555,9 @@
       <c r="T28">
         <v>229</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2013</v>
       </c>
@@ -14589,8 +14618,9 @@
       <c r="T29">
         <v>161.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U29" s="3"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2014</v>
       </c>
@@ -14651,8 +14681,9 @@
       <c r="T30">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2015</v>
       </c>
@@ -14713,8 +14744,9 @@
       <c r="T31">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2016</v>
       </c>
@@ -14775,8 +14807,9 @@
       <c r="T32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U32" s="3"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2017</v>
       </c>
@@ -14837,8 +14870,9 @@
       <c r="T33">
         <v>80.7</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U33" s="3"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2018</v>
       </c>
@@ -14899,8 +14933,9 @@
       <c r="T34">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2019</v>
       </c>
@@ -14961,8 +14996,9 @@
       <c r="T35">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U35" s="3"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -15023,8 +15059,9 @@
       <c r="T36">
         <v>30.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U36" s="3"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1993</v>
       </c>
@@ -15085,8 +15122,9 @@
       <c r="T37">
         <v>9380.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U37" s="3"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1995</v>
       </c>
@@ -15147,8 +15185,9 @@
       <c r="T38">
         <v>21160.7</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U38" s="3"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1997</v>
       </c>
@@ -15209,8 +15248,9 @@
       <c r="T39">
         <v>19421.7</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U39" s="3"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1999</v>
       </c>
@@ -15271,8 +15311,9 @@
       <c r="T40">
         <v>111182.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U40" s="3"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2000</v>
       </c>
@@ -15333,8 +15374,9 @@
       <c r="T41">
         <v>54613.2</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U41" s="3"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2001</v>
       </c>
@@ -15395,8 +15437,9 @@
       <c r="T42">
         <v>51516.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U42" s="3"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2004</v>
       </c>
@@ -15457,8 +15500,9 @@
       <c r="T43">
         <v>4906.1000000000004</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U43" s="3"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2005</v>
       </c>
@@ -15519,8 +15563,9 @@
       <c r="T44">
         <v>1067.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U44" s="3"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2006</v>
       </c>
@@ -15581,8 +15626,9 @@
       <c r="T45">
         <v>1151.8</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U45" s="3"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2007</v>
       </c>
@@ -15643,8 +15689,9 @@
       <c r="T46">
         <v>924.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U46" s="3"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2008</v>
       </c>
@@ -15705,8 +15752,9 @@
       <c r="T47">
         <v>2858.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U47" s="3"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2009</v>
       </c>
@@ -15767,8 +15815,9 @@
       <c r="T48">
         <v>2061.3000000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U48" s="3"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2010</v>
       </c>
@@ -15829,8 +15878,9 @@
       <c r="T49">
         <v>1394.1</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U49" s="3"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2011</v>
       </c>
@@ -15891,8 +15941,9 @@
       <c r="T50">
         <v>822</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U50" s="3"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2012</v>
       </c>
@@ -15953,8 +16004,9 @@
       <c r="T51">
         <v>700</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U51" s="3"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2013</v>
       </c>
@@ -16015,8 +16067,9 @@
       <c r="T52">
         <v>2000</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U52" s="3"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2014</v>
       </c>
@@ -16077,8 +16130,9 @@
       <c r="T53">
         <v>1000</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U53" s="3"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2015</v>
       </c>
@@ -16139,8 +16193,9 @@
       <c r="T54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U54" s="3"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2016</v>
       </c>
@@ -16201,8 +16256,9 @@
       <c r="T55">
         <v>3000</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U55" s="3"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2017</v>
       </c>
@@ -16263,8 +16319,9 @@
       <c r="T56">
         <v>6210</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U56" s="3"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2018</v>
       </c>
@@ -16325,16 +16382,17 @@
       <c r="T57">
         <v>6210</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>53</v>
+      <c r="U57" s="3"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>2001</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -16352,51 +16410,52 @@
         <v>-1</v>
       </c>
       <c r="I58">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J58">
-        <v>183240</v>
+        <v>459.99999999999994</v>
       </c>
       <c r="K58">
-        <v>500000</v>
+        <v>8690</v>
       </c>
       <c r="L58">
-        <v>112430</v>
+        <v>18920</v>
       </c>
       <c r="M58">
-        <v>50110</v>
+        <v>19290</v>
       </c>
       <c r="N58">
-        <v>34220</v>
+        <v>12700</v>
       </c>
       <c r="O58">
         <v>11410</v>
       </c>
       <c r="P58">
-        <v>3150</v>
+        <v>11900</v>
       </c>
       <c r="Q58">
-        <v>5980</v>
+        <v>5890</v>
       </c>
       <c r="R58">
-        <v>2230</v>
+        <v>1800</v>
       </c>
       <c r="S58">
-        <v>1640</v>
+        <v>300</v>
       </c>
       <c r="T58">
-        <v>6210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>54</v>
+        <v>200</v>
+      </c>
+      <c r="U58" s="3"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>2002</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -16414,101 +16473,921 @@
         <v>-1</v>
       </c>
       <c r="I59">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J59">
-        <v>183240</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>486550</v>
+        <v>620</v>
       </c>
       <c r="L59">
-        <v>113000</v>
+        <v>3490</v>
       </c>
       <c r="M59">
-        <v>50111</v>
+        <v>15010</v>
       </c>
       <c r="N59">
-        <v>34220</v>
+        <v>27539.999999999996</v>
       </c>
       <c r="O59">
-        <v>11410</v>
+        <v>25820</v>
       </c>
       <c r="P59">
-        <v>3150</v>
+        <v>30320</v>
       </c>
       <c r="Q59">
-        <v>5980</v>
+        <v>21920</v>
       </c>
       <c r="R59">
-        <v>2230</v>
+        <v>8610</v>
       </c>
       <c r="S59">
-        <v>1640</v>
+        <v>5680</v>
       </c>
       <c r="T59">
-        <v>6210</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+        <v>2360</v>
+      </c>
+      <c r="U59" s="3"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60">
+        <v>2003</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>-1</v>
+      </c>
+      <c r="I60">
+        <v>30</v>
+      </c>
+      <c r="J60">
+        <v>70</v>
+      </c>
+      <c r="K60">
+        <v>330</v>
+      </c>
+      <c r="L60">
+        <v>3750</v>
+      </c>
+      <c r="M60">
+        <v>10140</v>
+      </c>
+      <c r="N60">
+        <v>35630</v>
+      </c>
+      <c r="O60">
+        <v>78520</v>
+      </c>
+      <c r="P60">
+        <v>39450</v>
+      </c>
+      <c r="Q60">
+        <v>33260</v>
+      </c>
+      <c r="R60">
+        <v>11720</v>
+      </c>
+      <c r="S60">
+        <v>5440</v>
+      </c>
+      <c r="T60">
+        <v>4830</v>
+      </c>
+      <c r="U60" s="3"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>2004</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>-1</v>
+      </c>
+      <c r="I61">
+        <v>30</v>
+      </c>
+      <c r="J61">
+        <v>7370</v>
+      </c>
+      <c r="K61">
+        <v>6909.9999999999991</v>
+      </c>
+      <c r="L61">
+        <v>16850</v>
+      </c>
+      <c r="M61">
+        <v>43810</v>
+      </c>
+      <c r="N61">
+        <v>39920</v>
+      </c>
+      <c r="O61">
+        <v>44730</v>
+      </c>
+      <c r="P61">
+        <v>21600</v>
+      </c>
+      <c r="Q61">
+        <v>12360</v>
+      </c>
+      <c r="R61">
+        <v>14569.999999999998</v>
+      </c>
+      <c r="S61">
+        <v>4410</v>
+      </c>
+      <c r="T61">
+        <v>2680</v>
+      </c>
+      <c r="U61" s="3"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>2005</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>-1</v>
+      </c>
+      <c r="I62">
+        <v>30</v>
+      </c>
+      <c r="J62">
+        <v>1030</v>
+      </c>
+      <c r="K62">
+        <v>3720.0000000000005</v>
+      </c>
+      <c r="L62">
+        <v>12390</v>
+      </c>
+      <c r="M62">
+        <v>8470</v>
+      </c>
+      <c r="N62">
+        <v>16450</v>
+      </c>
+      <c r="O62">
+        <v>12410</v>
+      </c>
+      <c r="P62">
+        <v>4770</v>
+      </c>
+      <c r="Q62">
+        <v>2310</v>
+      </c>
+      <c r="R62">
+        <v>1000</v>
+      </c>
+      <c r="S62">
+        <v>459.99999999999994</v>
+      </c>
+      <c r="T62">
+        <v>409.99999999999994</v>
+      </c>
+      <c r="U62" s="3"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>2006</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>-1</v>
+      </c>
+      <c r="I63">
+        <v>30</v>
+      </c>
+      <c r="J63">
+        <v>5810</v>
+      </c>
+      <c r="K63">
+        <v>12310</v>
+      </c>
+      <c r="L63">
+        <v>28410.000000000004</v>
+      </c>
+      <c r="M63">
+        <v>19310</v>
+      </c>
+      <c r="N63">
+        <v>7590.0000000000009</v>
+      </c>
+      <c r="O63">
+        <v>4760</v>
+      </c>
+      <c r="P63">
+        <v>1030</v>
+      </c>
+      <c r="Q63">
+        <v>930.00000000000011</v>
+      </c>
+      <c r="R63">
+        <v>150</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63" s="3"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>2007</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>-1</v>
+      </c>
+      <c r="I64">
+        <v>30</v>
+      </c>
+      <c r="J64">
+        <v>4630</v>
+      </c>
+      <c r="K64">
+        <v>63820.000000000007</v>
+      </c>
+      <c r="L64">
+        <v>43090</v>
+      </c>
+      <c r="M64">
+        <v>22690</v>
+      </c>
+      <c r="N64">
+        <v>6409.9999999999991</v>
+      </c>
+      <c r="O64">
+        <v>4580</v>
+      </c>
+      <c r="P64">
+        <v>590</v>
+      </c>
+      <c r="Q64">
+        <v>490.00000000000006</v>
+      </c>
+      <c r="R64">
+        <v>60</v>
+      </c>
+      <c r="S64">
+        <v>40</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64" s="3"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>2008</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>-1</v>
+      </c>
+      <c r="I65">
+        <v>30</v>
+      </c>
+      <c r="J65">
+        <v>30110.000000000004</v>
+      </c>
+      <c r="K65">
+        <v>63679.999999999993</v>
+      </c>
+      <c r="L65">
+        <v>134290</v>
+      </c>
+      <c r="M65">
+        <v>71160</v>
+      </c>
+      <c r="N65">
+        <v>19910</v>
+      </c>
+      <c r="O65">
+        <v>12180</v>
+      </c>
+      <c r="P65">
+        <v>5040</v>
+      </c>
+      <c r="Q65">
+        <v>1130</v>
+      </c>
+      <c r="R65">
+        <v>360</v>
+      </c>
+      <c r="S65">
+        <v>190</v>
+      </c>
+      <c r="T65">
+        <v>240</v>
+      </c>
+      <c r="U65" s="3"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>2009</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>-1</v>
+      </c>
+      <c r="I66">
+        <v>30</v>
+      </c>
+      <c r="J66">
+        <v>32800</v>
+      </c>
+      <c r="K66">
+        <v>107900</v>
+      </c>
+      <c r="L66">
+        <v>141140</v>
+      </c>
+      <c r="M66">
+        <v>100840</v>
+      </c>
+      <c r="N66">
+        <v>24870</v>
+      </c>
+      <c r="O66">
+        <v>10890</v>
+      </c>
+      <c r="P66">
+        <v>2530</v>
+      </c>
+      <c r="Q66">
+        <v>560</v>
+      </c>
+      <c r="R66">
+        <v>250</v>
+      </c>
+      <c r="S66">
+        <v>140</v>
+      </c>
+      <c r="T66">
+        <v>30</v>
+      </c>
+      <c r="U66" s="3"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>2010</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>-1</v>
+      </c>
+      <c r="I67">
+        <v>30</v>
+      </c>
+      <c r="J67">
+        <v>31110.000000000004</v>
+      </c>
+      <c r="K67">
+        <v>104090.00000000001</v>
+      </c>
+      <c r="L67">
+        <v>150970</v>
+      </c>
+      <c r="M67">
+        <v>130930</v>
+      </c>
+      <c r="N67">
+        <v>51790</v>
+      </c>
+      <c r="O67">
+        <v>18110</v>
+      </c>
+      <c r="P67">
+        <v>5870</v>
+      </c>
+      <c r="Q67">
+        <v>2140</v>
+      </c>
+      <c r="R67">
+        <v>1120</v>
+      </c>
+      <c r="S67">
+        <v>580</v>
+      </c>
+      <c r="T67">
+        <v>790</v>
+      </c>
+      <c r="U67" s="3"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>2011</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>-1</v>
+      </c>
+      <c r="I68">
+        <v>30</v>
+      </c>
+      <c r="J68">
+        <v>27339.999999999996</v>
+      </c>
+      <c r="K68">
+        <v>102180</v>
+      </c>
+      <c r="L68">
+        <v>190190</v>
+      </c>
+      <c r="M68">
+        <v>170580</v>
+      </c>
+      <c r="N68">
+        <v>88090</v>
+      </c>
+      <c r="O68">
+        <v>31289.999999999996</v>
+      </c>
+      <c r="P68">
+        <v>6150</v>
+      </c>
+      <c r="Q68">
+        <v>2320</v>
+      </c>
+      <c r="R68">
+        <v>670</v>
+      </c>
+      <c r="S68">
+        <v>270</v>
+      </c>
+      <c r="T68">
+        <v>280</v>
+      </c>
+      <c r="U68" s="3"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>2012</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>-1</v>
+      </c>
+      <c r="I69">
+        <v>30</v>
+      </c>
+      <c r="J69">
+        <v>44050</v>
+      </c>
+      <c r="K69">
+        <v>182310</v>
+      </c>
+      <c r="L69">
+        <v>161840</v>
+      </c>
+      <c r="M69">
+        <v>82720</v>
+      </c>
+      <c r="N69">
+        <v>7500</v>
+      </c>
+      <c r="O69">
+        <v>620</v>
+      </c>
+      <c r="P69">
+        <v>430</v>
+      </c>
+      <c r="Q69">
+        <v>400</v>
+      </c>
+      <c r="R69">
+        <v>220.00000000000003</v>
+      </c>
+      <c r="S69">
+        <v>170</v>
+      </c>
+      <c r="T69">
+        <v>360</v>
+      </c>
+      <c r="U69" s="3"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>2013</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>-1</v>
+      </c>
+      <c r="I70">
+        <v>30</v>
+      </c>
+      <c r="J70">
+        <v>9730</v>
+      </c>
+      <c r="K70">
+        <v>115780</v>
+      </c>
+      <c r="L70">
+        <v>193820</v>
+      </c>
+      <c r="M70">
+        <v>78150</v>
+      </c>
+      <c r="N70">
+        <v>21770</v>
+      </c>
+      <c r="O70">
+        <v>8090.0000000000009</v>
+      </c>
+      <c r="P70">
+        <v>2160</v>
+      </c>
+      <c r="Q70">
+        <v>650</v>
+      </c>
+      <c r="R70">
+        <v>330</v>
+      </c>
+      <c r="S70">
+        <v>320</v>
+      </c>
+      <c r="T70">
+        <v>380</v>
+      </c>
+      <c r="U70" s="3"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>2014</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>-1</v>
+      </c>
+      <c r="I71">
+        <v>30</v>
+      </c>
+      <c r="J71">
+        <v>10790</v>
+      </c>
+      <c r="K71">
+        <v>72720</v>
+      </c>
+      <c r="L71">
+        <v>106859.99999999999</v>
+      </c>
+      <c r="M71">
+        <v>37000</v>
+      </c>
+      <c r="N71">
+        <v>9370</v>
+      </c>
+      <c r="O71">
+        <v>1610.0000000000002</v>
+      </c>
+      <c r="P71">
+        <v>240</v>
+      </c>
+      <c r="Q71">
+        <v>90</v>
+      </c>
+      <c r="R71">
+        <v>20</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71" s="3"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>2015</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>-1</v>
+      </c>
+      <c r="I72">
+        <v>30</v>
+      </c>
+      <c r="J72">
+        <v>9250</v>
+      </c>
+      <c r="K72">
+        <v>80330</v>
+      </c>
+      <c r="L72">
+        <v>113970</v>
+      </c>
+      <c r="M72">
+        <v>30400</v>
+      </c>
+      <c r="N72">
+        <v>6700</v>
+      </c>
+      <c r="O72">
+        <v>1019.9999999999999</v>
+      </c>
+      <c r="P72">
+        <v>310</v>
+      </c>
+      <c r="Q72">
+        <v>280</v>
+      </c>
+      <c r="R72">
+        <v>120</v>
+      </c>
+      <c r="S72">
+        <v>100</v>
+      </c>
+      <c r="T72">
+        <v>10</v>
+      </c>
+      <c r="U72" s="3"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A73">
         <v>-9999</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-      <c r="P60">
-        <v>0</v>
-      </c>
-      <c r="Q60">
-        <v>0</v>
-      </c>
-      <c r="R60">
-        <v>0</v>
-      </c>
-      <c r="S60">
-        <v>0</v>
-      </c>
-      <c r="T60">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>0</v>
+      </c>
+      <c r="T73">
         <v>0</v>
       </c>
     </row>
@@ -17043,7 +17922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L107" workbookViewId="0">
+    <sheetView topLeftCell="L107" workbookViewId="0">
       <selection activeCell="U1" sqref="U1:BA1048576"/>
     </sheetView>
   </sheetViews>
@@ -17173,7 +18052,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -17235,7 +18114,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -17297,7 +18176,7 @@
         <v>0.18</v>
       </c>
       <c r="T4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -17359,7 +18238,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -17421,7 +18300,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -17483,7 +18362,7 @@
         <v>1.28</v>
       </c>
       <c r="T7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -17545,7 +18424,7 @@
         <v>1.28</v>
       </c>
       <c r="T8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
@@ -17607,7 +18486,7 @@
         <v>1</v>
       </c>
       <c r="T9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
@@ -17669,7 +18548,7 @@
         <v>1.28</v>
       </c>
       <c r="T10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -17731,7 +18610,7 @@
         <v>1.28</v>
       </c>
       <c r="T11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -17793,7 +18672,7 @@
         <v>1.24</v>
       </c>
       <c r="T12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
@@ -17855,7 +18734,7 @@
         <v>1.24</v>
       </c>
       <c r="T13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
@@ -17917,7 +18796,7 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -17979,7 +18858,7 @@
         <v>1.24</v>
       </c>
       <c r="T15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
@@ -18041,7 +18920,7 @@
         <v>1.24</v>
       </c>
       <c r="T16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
@@ -18103,7 +18982,7 @@
         <v>1.44</v>
       </c>
       <c r="T17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -18165,7 +19044,7 @@
         <v>1.44</v>
       </c>
       <c r="T18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
@@ -18227,7 +19106,7 @@
         <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -18289,7 +19168,7 @@
         <v>1.44</v>
       </c>
       <c r="T20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
@@ -18351,7 +19230,7 @@
         <v>1.44</v>
       </c>
       <c r="T21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
@@ -18413,7 +19292,7 @@
         <v>1.53</v>
       </c>
       <c r="T22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
@@ -18475,7 +19354,7 @@
         <v>1.53</v>
       </c>
       <c r="T23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
@@ -18537,7 +19416,7 @@
         <v>1</v>
       </c>
       <c r="T24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
@@ -18599,7 +19478,7 @@
         <v>1.53</v>
       </c>
       <c r="T25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
@@ -18661,7 +19540,7 @@
         <v>1.53</v>
       </c>
       <c r="T26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -18723,7 +19602,7 @@
         <v>1.48</v>
       </c>
       <c r="T27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
@@ -18785,7 +19664,7 @@
         <v>1.48</v>
       </c>
       <c r="T28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
@@ -18847,7 +19726,7 @@
         <v>1</v>
       </c>
       <c r="T29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
@@ -18909,7 +19788,7 @@
         <v>1.48</v>
       </c>
       <c r="T30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
@@ -18971,7 +19850,7 @@
         <v>1.48</v>
       </c>
       <c r="T31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
@@ -19033,7 +19912,7 @@
         <v>1.56</v>
       </c>
       <c r="T32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.35">
@@ -19095,7 +19974,7 @@
         <v>1.56</v>
       </c>
       <c r="T33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
@@ -19157,7 +20036,7 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
@@ -19219,7 +20098,7 @@
         <v>1.56</v>
       </c>
       <c r="T35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
@@ -19281,7 +20160,7 @@
         <v>1.56</v>
       </c>
       <c r="T36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
@@ -19343,7 +20222,7 @@
         <v>1.72</v>
       </c>
       <c r="T37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
@@ -19405,7 +20284,7 @@
         <v>1.72</v>
       </c>
       <c r="T38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
@@ -19467,7 +20346,7 @@
         <v>1</v>
       </c>
       <c r="T39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
@@ -19529,7 +20408,7 @@
         <v>1.72</v>
       </c>
       <c r="T40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
@@ -19591,7 +20470,7 @@
         <v>1.72</v>
       </c>
       <c r="T41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
@@ -19653,7 +20532,7 @@
         <v>1.75</v>
       </c>
       <c r="T42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
@@ -19715,7 +20594,7 @@
         <v>1.75</v>
       </c>
       <c r="T43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
@@ -19777,7 +20656,7 @@
         <v>1</v>
       </c>
       <c r="T44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
@@ -19839,7 +20718,7 @@
         <v>1.75</v>
       </c>
       <c r="T45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.35">
@@ -19901,7 +20780,7 @@
         <v>1.75</v>
       </c>
       <c r="T46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.35">
@@ -19963,7 +20842,7 @@
         <v>1.37</v>
       </c>
       <c r="T47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.35">
@@ -20025,7 +20904,7 @@
         <v>1.37</v>
       </c>
       <c r="T48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.35">
@@ -20087,7 +20966,7 @@
         <v>1</v>
       </c>
       <c r="T49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
@@ -20149,7 +21028,7 @@
         <v>1.37</v>
       </c>
       <c r="T50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.35">
@@ -20211,7 +21090,7 @@
         <v>1.37</v>
       </c>
       <c r="T51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.35">
@@ -20273,7 +21152,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="T52" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.35">
@@ -20335,7 +21214,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="T53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.35">
@@ -20397,7 +21276,7 @@
         <v>1</v>
       </c>
       <c r="T54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
@@ -20459,7 +21338,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="T55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.35">
@@ -20521,7 +21400,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="T56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.35">
@@ -20583,7 +21462,7 @@
         <v>1.02</v>
       </c>
       <c r="T57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.35">
@@ -20645,7 +21524,7 @@
         <v>1.02</v>
       </c>
       <c r="T58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.35">
@@ -20707,7 +21586,7 @@
         <v>1</v>
       </c>
       <c r="T59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.35">
@@ -20769,7 +21648,7 @@
         <v>1.02</v>
       </c>
       <c r="T60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.35">
@@ -20831,7 +21710,7 @@
         <v>1.02</v>
       </c>
       <c r="T61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.35">
@@ -20893,7 +21772,7 @@
         <v>1.18</v>
       </c>
       <c r="T62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.35">
@@ -20955,7 +21834,7 @@
         <v>1.18</v>
       </c>
       <c r="T63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.35">
@@ -21017,7 +21896,7 @@
         <v>1</v>
       </c>
       <c r="T64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.35">
@@ -21079,7 +21958,7 @@
         <v>1.18</v>
       </c>
       <c r="T65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.35">
@@ -21141,7 +22020,7 @@
         <v>1.18</v>
       </c>
       <c r="T66" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.35">
@@ -21203,7 +22082,7 @@
         <v>1.55</v>
       </c>
       <c r="T67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.35">
@@ -21265,7 +22144,7 @@
         <v>1.55</v>
       </c>
       <c r="T68" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.35">
@@ -21327,7 +22206,7 @@
         <v>1</v>
       </c>
       <c r="T69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.35">
@@ -21389,7 +22268,7 @@
         <v>1.55</v>
       </c>
       <c r="T70" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.35">
@@ -21451,7 +22330,7 @@
         <v>1.55</v>
       </c>
       <c r="T71" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.35">
@@ -21513,7 +22392,7 @@
         <v>1.54</v>
       </c>
       <c r="T72" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.35">
@@ -21575,7 +22454,7 @@
         <v>1.54</v>
       </c>
       <c r="T73" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.35">
@@ -21637,7 +22516,7 @@
         <v>1</v>
       </c>
       <c r="T74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.35">
@@ -21699,7 +22578,7 @@
         <v>1.54</v>
       </c>
       <c r="T75" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.35">
@@ -21761,7 +22640,7 @@
         <v>1.54</v>
       </c>
       <c r="T76" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.35">
@@ -21823,7 +22702,7 @@
         <v>2.02</v>
       </c>
       <c r="T77" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.35">
@@ -21885,7 +22764,7 @@
         <v>2.02</v>
       </c>
       <c r="T78" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.35">
@@ -21947,7 +22826,7 @@
         <v>1</v>
       </c>
       <c r="T79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.35">
@@ -22009,7 +22888,7 @@
         <v>2.02</v>
       </c>
       <c r="T80" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.35">
@@ -22071,7 +22950,7 @@
         <v>2.02</v>
       </c>
       <c r="T81" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.35">
@@ -22133,7 +23012,7 @@
         <v>1.63</v>
       </c>
       <c r="T82" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.35">
@@ -22195,7 +23074,7 @@
         <v>1.63</v>
       </c>
       <c r="T83" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.35">
@@ -22257,7 +23136,7 @@
         <v>1</v>
       </c>
       <c r="T84" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.35">
@@ -22319,7 +23198,7 @@
         <v>1.63</v>
       </c>
       <c r="T85" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.35">
@@ -22381,7 +23260,7 @@
         <v>1.63</v>
       </c>
       <c r="T86" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.35">
@@ -22443,7 +23322,7 @@
         <v>1.6</v>
       </c>
       <c r="T87" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.35">
@@ -22505,7 +23384,7 @@
         <v>1.6</v>
       </c>
       <c r="T88" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.35">
@@ -22567,7 +23446,7 @@
         <v>0.18</v>
       </c>
       <c r="T89" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.35">
@@ -22629,7 +23508,7 @@
         <v>1.6</v>
       </c>
       <c r="T90" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.35">
@@ -22691,7 +23570,7 @@
         <v>1.6</v>
       </c>
       <c r="T91" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.35">
@@ -22753,7 +23632,7 @@
         <v>1.25</v>
       </c>
       <c r="T92" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.35">
@@ -22815,7 +23694,7 @@
         <v>1.25</v>
       </c>
       <c r="T93" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.35">
@@ -22877,7 +23756,7 @@
         <v>0.18</v>
       </c>
       <c r="T94" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.35">
@@ -22939,7 +23818,7 @@
         <v>1.25</v>
       </c>
       <c r="T95" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.35">
@@ -23001,7 +23880,7 @@
         <v>1.25</v>
       </c>
       <c r="T96" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.35">
@@ -23063,7 +23942,7 @@
         <v>1.49</v>
       </c>
       <c r="T97" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.35">
@@ -23125,7 +24004,7 @@
         <v>1.49</v>
       </c>
       <c r="T98" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.35">
@@ -23187,7 +24066,7 @@
         <v>0.18</v>
       </c>
       <c r="T99" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.35">
@@ -23249,7 +24128,7 @@
         <v>1.49</v>
       </c>
       <c r="T100" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.35">
@@ -23311,7 +24190,7 @@
         <v>1.49</v>
       </c>
       <c r="T101" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.35">
@@ -23373,7 +24252,7 @@
         <v>1.68</v>
       </c>
       <c r="T102" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.35">
@@ -23435,7 +24314,7 @@
         <v>1.68</v>
       </c>
       <c r="T103" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.35">
@@ -23497,7 +24376,7 @@
         <v>0.18</v>
       </c>
       <c r="T104" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.35">
@@ -23559,7 +24438,7 @@
         <v>1.68</v>
       </c>
       <c r="T105" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.35">
@@ -23621,7 +24500,7 @@
         <v>1.68</v>
       </c>
       <c r="T106" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.35">
@@ -23683,7 +24562,7 @@
         <v>1.48</v>
       </c>
       <c r="T107" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.35">
@@ -23745,7 +24624,7 @@
         <v>1.48</v>
       </c>
       <c r="T108" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.35">
@@ -23807,7 +24686,7 @@
         <v>0.18</v>
       </c>
       <c r="T109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.35">
@@ -23869,7 +24748,7 @@
         <v>1.48</v>
       </c>
       <c r="T110" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.35">
@@ -23931,7 +24810,7 @@
         <v>1.48</v>
       </c>
       <c r="T111" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.35">
@@ -23993,7 +24872,7 @@
         <v>1.52</v>
       </c>
       <c r="T112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.35">
@@ -24055,7 +24934,7 @@
         <v>1.52</v>
       </c>
       <c r="T113" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.35">
@@ -24117,7 +24996,7 @@
         <v>0.18</v>
       </c>
       <c r="T114" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.35">
@@ -24179,7 +25058,7 @@
         <v>1.52</v>
       </c>
       <c r="T115" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.35">
@@ -24241,7 +25120,7 @@
         <v>1.52</v>
       </c>
       <c r="T116" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.35">
@@ -24303,7 +25182,7 @@
         <v>1.57</v>
       </c>
       <c r="T117" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.35">
@@ -24365,7 +25244,7 @@
         <v>1.57</v>
       </c>
       <c r="T118" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.35">
@@ -24427,7 +25306,7 @@
         <v>0.18</v>
       </c>
       <c r="T119" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.35">
@@ -24489,7 +25368,7 @@
         <v>1.57</v>
       </c>
       <c r="T120" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.35">
@@ -24551,7 +25430,7 @@
         <v>1.57</v>
       </c>
       <c r="T121" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.35">
@@ -24613,7 +25492,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="T122" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.35">
@@ -24675,7 +25554,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="T123" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.35">
@@ -24737,7 +25616,7 @@
         <v>0.18</v>
       </c>
       <c r="T124" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.35">
@@ -24799,7 +25678,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="T125" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.35">
@@ -24861,7 +25740,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="T126" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.35">
@@ -24923,7 +25802,7 @@
         <v>2.09</v>
       </c>
       <c r="T127" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.35">
@@ -24985,7 +25864,7 @@
         <v>2.09</v>
       </c>
       <c r="T128" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.35">
@@ -25047,7 +25926,7 @@
         <v>0.18</v>
       </c>
       <c r="T129" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.35">
@@ -25109,7 +25988,7 @@
         <v>2.09</v>
       </c>
       <c r="T130" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.35">
@@ -25171,7 +26050,7 @@
         <v>2.09</v>
       </c>
       <c r="T131" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.35">
@@ -25233,7 +26112,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="T132" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.35">
@@ -25295,7 +26174,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="T133" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.35">
@@ -25357,7 +26236,7 @@
         <v>0.18</v>
       </c>
       <c r="T134" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.35">
@@ -25419,7 +26298,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="T135" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.35">
@@ -25481,7 +26360,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="T136" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.35">
@@ -25543,7 +26422,7 @@
         <v>3</v>
       </c>
       <c r="T137" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.35">
@@ -25605,7 +26484,7 @@
         <v>3</v>
       </c>
       <c r="T138" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.35">
@@ -25667,7 +26546,7 @@
         <v>0.18</v>
       </c>
       <c r="T139" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.35">
@@ -25729,7 +26608,7 @@
         <v>3</v>
       </c>
       <c r="T140" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.35">
@@ -25791,7 +26670,7 @@
         <v>3</v>
       </c>
       <c r="T141" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.35">
@@ -25853,7 +26732,7 @@
         <v>2.11</v>
       </c>
       <c r="T142" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.35">
@@ -25915,7 +26794,7 @@
         <v>2.11</v>
       </c>
       <c r="T143" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.35">
@@ -25977,7 +26856,7 @@
         <v>0.18</v>
       </c>
       <c r="T144" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.35">
@@ -26039,7 +26918,7 @@
         <v>2.11</v>
       </c>
       <c r="T145" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.35">
@@ -26101,7 +26980,7 @@
         <v>2.11</v>
       </c>
       <c r="T146" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>